<commit_message>
feat: added multiple categories feature
</commit_message>
<xml_diff>
--- a/web/public/sheets/importacao-de-produtos.xlsx
+++ b/web/public/sheets/importacao-de-produtos.xlsx
@@ -25,7 +25,7 @@
     <t>Preço Promocional</t>
   </si>
   <si>
-    <t>Categoria</t>
+    <t>Categorias</t>
   </si>
   <si>
     <t>Visível no catálogo</t>
@@ -40,7 +40,7 @@
     <t>Descrição para o catálogo</t>
   </si>
   <si>
-    <t>Categoria do produto</t>
+    <t>Categoria 1,Categoria 2</t>
   </si>
   <si>
     <t>S</t>

</xml_diff>